<commit_message>
Updated HEE and GTM shapefiles
</commit_message>
<xml_diff>
--- a/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_CBM_2020.xlsx
+++ b/CDMO_Automation/00_Annual_Update/Updated_reserve_var_sheets/Reserve_Level_Plotting_Variables_CBM_2020.xlsx
@@ -1483,7 +1483,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-77.2453</v>
+        <v>-77.245</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>-76.7708837726</v>
@@ -1503,7 +1503,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37.791</v>
+        <v>37.7912</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>38.7091447287</v>
@@ -1521,7 +1521,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-75.283</v>
+        <v>-75.2824</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>-76.653188493</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39.8499</v>
+        <v>39.85</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>38.8019367381</v>

</xml_diff>